<commit_message>
fixed modification & renouveler
</commit_message>
<xml_diff>
--- a/Cosider.xlsx
+++ b/Cosider.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="52">
   <si>
     <t>Matricule</t>
   </si>
@@ -73,79 +73,58 @@
     <t>Duree Essais</t>
   </si>
   <si>
-    <t>Brouri Toufik</t>
-  </si>
-  <si>
-    <t>Akbou</t>
-  </si>
-  <si>
-    <t>LHARA AIT BRAHEM</t>
-  </si>
-  <si>
-    <t>Toufik2027NoYes</t>
-  </si>
-  <si>
-    <t>T133</t>
-  </si>
-  <si>
-    <t>Chemini Bejaia</t>
-  </si>
-  <si>
-    <t>Zermani Sofiane</t>
-  </si>
-  <si>
-    <t>49000</t>
-  </si>
-  <si>
-    <t>part</t>
-  </si>
-  <si>
-    <t>Careleur</t>
-  </si>
-  <si>
-    <t>12</t>
+    <t xml:space="preserve">Bouatoura Lyes </t>
+  </si>
+  <si>
+    <t>Safi</t>
+  </si>
+  <si>
+    <t>Ben Aknoun</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>T134</t>
+  </si>
+  <si>
+    <t>Azazga Tizi Ouzou</t>
+  </si>
+  <si>
+    <t>Zerrouk Ahmed</t>
+  </si>
+  <si>
+    <t>4500Da</t>
+  </si>
+  <si>
+    <t>plein</t>
+  </si>
+  <si>
+    <t>medecin</t>
+  </si>
+  <si>
+    <t>2</t>
   </si>
   <si>
     <t>B</t>
   </si>
   <si>
-    <t>Chantier</t>
-  </si>
-  <si>
-    <t>Cat C</t>
-  </si>
-  <si>
-    <t>50 jours</t>
-  </si>
-  <si>
-    <t>SALIM BOUMECHRA</t>
-  </si>
-  <si>
-    <t>Bougarra</t>
-  </si>
-  <si>
-    <t>emirats</t>
-  </si>
-  <si>
-    <t>Contract</t>
-  </si>
-  <si>
-    <t>T134</t>
-  </si>
-  <si>
-    <t>Azazga Tizi Ouzou</t>
-  </si>
-  <si>
-    <t>Zerrouk Ahmed</t>
-  </si>
-  <si>
-    <t>41000 DA</t>
-  </si>
-  <si>
-    <t>plein</t>
-  </si>
-  <si>
-    <t>Peintre</t>
+    <t>support</t>
+  </si>
+  <si>
+    <t>Cat E</t>
+  </si>
+  <si>
+    <t>4 mois</t>
+  </si>
+  <si>
+    <t>4700Da</t>
+  </si>
+  <si>
+    <t>partiel</t>
+  </si>
+  <si>
+    <t>pilote</t>
   </si>
   <si>
     <t>1</t>
@@ -154,22 +133,40 @@
     <t>A</t>
   </si>
   <si>
-    <t>Travaux</t>
+    <t>Tech</t>
   </si>
   <si>
     <t>Cat A</t>
   </si>
   <si>
-    <t>45 jours</t>
-  </si>
-  <si>
-    <t>T131</t>
-  </si>
-  <si>
-    <t>Aokas Bejaia</t>
-  </si>
-  <si>
-    <t>Tamazouzt Kamel</t>
+    <t>6 mois</t>
+  </si>
+  <si>
+    <t>Bouatoura Lyacine</t>
+  </si>
+  <si>
+    <t>Alger</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>4800Da</t>
+  </si>
+  <si>
+    <t>copilote</t>
+  </si>
+  <si>
+    <t>Technique</t>
+  </si>
+  <si>
+    <t>Cat B</t>
+  </si>
+  <si>
+    <t>9 mois</t>
+  </si>
+  <si>
+    <t>49000Da</t>
   </si>
 </sst>
 </file>
@@ -547,7 +544,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T4"/>
+  <dimension ref="A1:T12"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="20" width="15" customWidth="1"/>
@@ -617,13 +614,13 @@
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>129</v>
+        <v>197</v>
       </c>
       <c r="B2" t="s">
         <v>20</v>
       </c>
       <c r="C2" s="1">
-        <v>31100</v>
+        <v>33599</v>
       </c>
       <c r="D2" t="s">
         <v>21</v>
@@ -635,10 +632,10 @@
         <v>23</v>
       </c>
       <c r="G2" s="1">
-        <v>44545</v>
+        <v>44556</v>
       </c>
       <c r="H2" s="1">
-        <v>46752</v>
+        <v>62088</v>
       </c>
       <c r="I2" t="s">
         <v>24</v>
@@ -650,7 +647,7 @@
         <v>26</v>
       </c>
       <c r="L2">
-        <v>49000</v>
+        <v>45000</v>
       </c>
       <c r="M2" t="s">
         <v>27</v>
@@ -679,126 +676,622 @@
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>129</v>
+        <v>197</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="C3" s="1">
-        <v>32151</v>
+        <v>33599</v>
       </c>
       <c r="D3" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="E3" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="F3" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="G3" s="1">
-        <v>44542</v>
+        <v>46017</v>
       </c>
       <c r="H3" s="1">
-        <v>44907</v>
+        <v>62088</v>
       </c>
       <c r="I3" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="J3" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="K3" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="L3">
-        <v>41000</v>
+        <v>45000</v>
       </c>
       <c r="M3" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="N3" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="O3" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="P3" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="Q3" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="R3" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="S3" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="T3" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>129</v>
+        <v>197</v>
       </c>
       <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="1">
+        <v>33599</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="1">
+        <v>44556</v>
+      </c>
+      <c r="H4" s="1">
+        <v>44921</v>
+      </c>
+      <c r="I4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" t="s">
+        <v>25</v>
+      </c>
+      <c r="K4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L4">
+        <v>47000</v>
+      </c>
+      <c r="M4" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="1">
-        <v>32151</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="N4" t="s">
         <v>36</v>
       </c>
-      <c r="E4" t="s">
+      <c r="O4" t="s">
         <v>37</v>
       </c>
-      <c r="F4" t="s">
+      <c r="P4" t="s">
         <v>38</v>
       </c>
-      <c r="G4" s="1">
-        <v>44542</v>
-      </c>
-      <c r="H4" s="1">
-        <v>44907</v>
-      </c>
-      <c r="I4" t="s">
+      <c r="Q4" t="s">
+        <v>39</v>
+      </c>
+      <c r="R4" t="s">
+        <v>40</v>
+      </c>
+      <c r="S4" t="s">
+        <v>41</v>
+      </c>
+      <c r="T4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>197</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="1">
+        <v>33599</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="1">
+        <v>44556</v>
+      </c>
+      <c r="H5" s="1">
+        <v>45652</v>
+      </c>
+      <c r="I5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K5" t="s">
+        <v>26</v>
+      </c>
+      <c r="L5">
+        <v>47000</v>
+      </c>
+      <c r="M5" t="s">
+        <v>35</v>
+      </c>
+      <c r="N5" t="s">
+        <v>36</v>
+      </c>
+      <c r="O5" t="s">
+        <v>37</v>
+      </c>
+      <c r="P5" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>39</v>
+      </c>
+      <c r="R5" t="s">
+        <v>40</v>
+      </c>
+      <c r="S5" t="s">
+        <v>41</v>
+      </c>
+      <c r="T5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>197</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="1">
+        <v>33599</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="1">
+        <v>44556</v>
+      </c>
+      <c r="H6" s="1">
+        <v>44921</v>
+      </c>
+      <c r="I6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J6" t="s">
+        <v>25</v>
+      </c>
+      <c r="K6" t="s">
+        <v>26</v>
+      </c>
+      <c r="L6">
+        <v>47000</v>
+      </c>
+      <c r="M6" t="s">
+        <v>35</v>
+      </c>
+      <c r="N6" t="s">
+        <v>36</v>
+      </c>
+      <c r="O6" t="s">
+        <v>37</v>
+      </c>
+      <c r="P6" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>39</v>
+      </c>
+      <c r="R6" t="s">
+        <v>40</v>
+      </c>
+      <c r="S6" t="s">
+        <v>41</v>
+      </c>
+      <c r="T6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>197</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="1">
+        <v>33599</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="1">
+        <v>44556</v>
+      </c>
+      <c r="H7" s="1">
+        <v>45286</v>
+      </c>
+      <c r="I7" t="s">
+        <v>24</v>
+      </c>
+      <c r="J7" t="s">
+        <v>25</v>
+      </c>
+      <c r="K7" t="s">
+        <v>26</v>
+      </c>
+      <c r="L7">
+        <v>47000</v>
+      </c>
+      <c r="M7" t="s">
+        <v>35</v>
+      </c>
+      <c r="N7" t="s">
+        <v>36</v>
+      </c>
+      <c r="O7" t="s">
+        <v>37</v>
+      </c>
+      <c r="P7" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>39</v>
+      </c>
+      <c r="R7" t="s">
+        <v>40</v>
+      </c>
+      <c r="S7" t="s">
+        <v>41</v>
+      </c>
+      <c r="T7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>197</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="1">
+        <v>33600</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="1">
+        <v>44556</v>
+      </c>
+      <c r="H8" s="1">
+        <v>45286</v>
+      </c>
+      <c r="I8" t="s">
+        <v>24</v>
+      </c>
+      <c r="J8" t="s">
+        <v>25</v>
+      </c>
+      <c r="K8" t="s">
+        <v>26</v>
+      </c>
+      <c r="L8">
+        <v>47000</v>
+      </c>
+      <c r="M8" t="s">
+        <v>35</v>
+      </c>
+      <c r="N8" t="s">
+        <v>36</v>
+      </c>
+      <c r="O8" t="s">
+        <v>37</v>
+      </c>
+      <c r="P8" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>39</v>
+      </c>
+      <c r="R8" t="s">
+        <v>40</v>
+      </c>
+      <c r="S8" t="s">
+        <v>41</v>
+      </c>
+      <c r="T8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>197</v>
+      </c>
+      <c r="B9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="1">
+        <v>33603</v>
+      </c>
+      <c r="D9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" s="1">
+        <v>44556</v>
+      </c>
+      <c r="H9" s="1">
+        <v>47478</v>
+      </c>
+      <c r="I9" t="s">
+        <v>24</v>
+      </c>
+      <c r="J9" t="s">
+        <v>25</v>
+      </c>
+      <c r="K9" t="s">
+        <v>26</v>
+      </c>
+      <c r="L9">
+        <v>47000</v>
+      </c>
+      <c r="M9" t="s">
+        <v>35</v>
+      </c>
+      <c r="N9" t="s">
+        <v>36</v>
+      </c>
+      <c r="O9" t="s">
+        <v>37</v>
+      </c>
+      <c r="P9" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>39</v>
+      </c>
+      <c r="R9" t="s">
+        <v>40</v>
+      </c>
+      <c r="S9" t="s">
+        <v>41</v>
+      </c>
+      <c r="T9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>197</v>
+      </c>
+      <c r="B10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="1">
+        <v>33603</v>
+      </c>
+      <c r="D10" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" t="s">
+        <v>45</v>
+      </c>
+      <c r="G10" s="1">
+        <v>44191</v>
+      </c>
+      <c r="H10" s="1">
+        <v>47478</v>
+      </c>
+      <c r="I10" t="s">
+        <v>24</v>
+      </c>
+      <c r="J10" t="s">
+        <v>25</v>
+      </c>
+      <c r="K10" t="s">
+        <v>26</v>
+      </c>
+      <c r="L10">
+        <v>48000</v>
+      </c>
+      <c r="M10" t="s">
+        <v>46</v>
+      </c>
+      <c r="N10" t="s">
+        <v>28</v>
+      </c>
+      <c r="O10" t="s">
+        <v>47</v>
+      </c>
+      <c r="P10" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>31</v>
+      </c>
+      <c r="R10" t="s">
+        <v>48</v>
+      </c>
+      <c r="S10" t="s">
+        <v>49</v>
+      </c>
+      <c r="T10" t="s">
         <v>50</v>
       </c>
-      <c r="J4" t="s">
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>197</v>
+      </c>
+      <c r="B11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="1">
+        <v>33603</v>
+      </c>
+      <c r="D11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" t="s">
+        <v>45</v>
+      </c>
+      <c r="G11" s="1">
+        <v>44191</v>
+      </c>
+      <c r="H11" s="1">
+        <v>47478</v>
+      </c>
+      <c r="I11" t="s">
+        <v>24</v>
+      </c>
+      <c r="J11" t="s">
+        <v>25</v>
+      </c>
+      <c r="K11" t="s">
+        <v>26</v>
+      </c>
+      <c r="L11">
+        <v>48000</v>
+      </c>
+      <c r="M11" t="s">
         <v>51</v>
       </c>
-      <c r="K4" t="s">
-        <v>52</v>
-      </c>
-      <c r="L4">
-        <v>41000</v>
-      </c>
-      <c r="M4" t="s">
-        <v>42</v>
-      </c>
-      <c r="N4" t="s">
+      <c r="N11" t="s">
+        <v>28</v>
+      </c>
+      <c r="O11" t="s">
+        <v>47</v>
+      </c>
+      <c r="P11" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>31</v>
+      </c>
+      <c r="R11" t="s">
+        <v>48</v>
+      </c>
+      <c r="S11" t="s">
+        <v>49</v>
+      </c>
+      <c r="T11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>197</v>
+      </c>
+      <c r="B12" t="s">
         <v>43</v>
       </c>
-      <c r="O4" t="s">
+      <c r="C12" s="1">
+        <v>33603</v>
+      </c>
+      <c r="D12" t="s">
         <v>44</v>
       </c>
-      <c r="P4" t="s">
+      <c r="E12" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" t="s">
         <v>45</v>
       </c>
-      <c r="Q4" t="s">
-        <v>46</v>
-      </c>
-      <c r="R4" t="s">
+      <c r="G12" s="1">
+        <v>44191</v>
+      </c>
+      <c r="H12" s="1">
+        <v>47478</v>
+      </c>
+      <c r="I12" t="s">
+        <v>24</v>
+      </c>
+      <c r="J12" t="s">
+        <v>25</v>
+      </c>
+      <c r="K12" t="s">
+        <v>26</v>
+      </c>
+      <c r="L12">
+        <v>49000</v>
+      </c>
+      <c r="M12" t="s">
+        <v>51</v>
+      </c>
+      <c r="N12" t="s">
+        <v>28</v>
+      </c>
+      <c r="O12" t="s">
         <v>47</v>
       </c>
-      <c r="S4" t="s">
+      <c r="P12" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>31</v>
+      </c>
+      <c r="R12" t="s">
         <v>48</v>
       </c>
-      <c r="T4" t="s">
+      <c r="S12" t="s">
         <v>49</v>
+      </c>
+      <c r="T12" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>